<commit_message>
Some mistakes changed - multiple spaces deleted - redundancy added - results view updated
</commit_message>
<xml_diff>
--- a/cp_1/results_for_bigrams_with_spaces_onestep.xlsx
+++ b/cp_1/results_for_bigrams_with_spaces_onestep.xlsx
@@ -428,7 +428,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>4e-05</v>
+        <v>1e-05</v>
       </c>
       <c r="D1" t="inlineStr">
         <is>
@@ -436,7 +436,7 @@
         </is>
       </c>
       <c r="E1" t="n">
-        <v>0.00329</v>
+        <v>0.00349</v>
       </c>
       <c r="G1" t="inlineStr">
         <is>
@@ -444,7 +444,7 @@
         </is>
       </c>
       <c r="H1" t="n">
-        <v>0.00026</v>
+        <v>0.00025</v>
       </c>
       <c r="J1" t="inlineStr">
         <is>
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="K1" t="n">
-        <v>0.00218</v>
+        <v>0.00221</v>
       </c>
       <c r="M1" t="inlineStr">
         <is>
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="N1" t="n">
-        <v>0.00817</v>
+        <v>0.00827</v>
       </c>
       <c r="P1" t="inlineStr">
         <is>
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="W1" t="n">
-        <v>2e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="2">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.00061</v>
+        <v>0.00063</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.00067</v>
+        <v>0.00068</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="W2" t="n">
-        <v>4e-05</v>
+        <v>5e-05</v>
       </c>
     </row>
     <row r="3">
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.00369</v>
+        <v>0.00379</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -568,7 +568,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.00087</v>
+        <v>0.00095</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
         </is>
       </c>
       <c r="T3" t="n">
-        <v>2e-05</v>
+        <v>3e-05</v>
       </c>
       <c r="V3" t="inlineStr">
         <is>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>0.00096</v>
+        <v>0.00099</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.00182</v>
+        <v>0.00183</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -708,7 +708,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>0.00181</v>
+        <v>0.00183</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -766,7 +766,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.00418</v>
+        <v>0.00421</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -774,7 +774,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>0.00249</v>
+        <v>0.00248</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>0.00306</v>
+        <v>0.00309</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
@@ -790,7 +790,7 @@
         </is>
       </c>
       <c r="N6" t="n">
-        <v>0.00481</v>
+        <v>0.00484</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
@@ -798,7 +798,7 @@
         </is>
       </c>
       <c r="Q6" t="n">
-        <v>2e-05</v>
+        <v>3e-05</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="T6" t="n">
-        <v>0.00175</v>
+        <v>0.00184</v>
       </c>
       <c r="V6" t="inlineStr">
         <is>
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.00457</v>
+        <v>0.00451</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -906,7 +906,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>0.00171</v>
+        <v>0.00181</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -946,7 +946,7 @@
         </is>
       </c>
       <c r="W8" t="n">
-        <v>0.00021</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="9">
@@ -956,7 +956,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5e-05</v>
+        <v>0.0001</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>0.00035</v>
+        <v>0.00037</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -980,7 +980,7 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>0.00244</v>
+        <v>0.00318</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
@@ -1004,7 +1004,7 @@
         </is>
       </c>
       <c r="T9" t="n">
-        <v>0.00144</v>
+        <v>0.00145</v>
       </c>
       <c r="V9" t="inlineStr">
         <is>
@@ -1088,7 +1088,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.00452</v>
+        <v>0.00459</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1104,7 +1104,7 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>0.00167</v>
+        <v>0.0017</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>9.000000000000001e-05</v>
+        <v>0.00011</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
@@ -1120,7 +1120,7 @@
         </is>
       </c>
       <c r="N11" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>8.000000000000001e-05</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
@@ -1144,7 +1144,7 @@
         </is>
       </c>
       <c r="W11" t="n">
-        <v>0.00107</v>
+        <v>0.00114</v>
       </c>
     </row>
     <row r="12">
@@ -1154,7 +1154,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.00779</v>
+        <v>0.0078</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.00085</v>
+        <v>0.00087</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>0.00554</v>
+        <v>0.00555</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>0.00025</v>
+        <v>0.00019</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
@@ -1220,7 +1220,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.00242</v>
+        <v>0.00243</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1236,7 +1236,7 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>0.00242</v>
+        <v>0.00244</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1286,7 +1286,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0032</v>
+        <v>0.00499</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1294,7 +1294,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.00189</v>
+        <v>0.00188</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>0.00383</v>
+        <v>0.00384</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="K14" t="n">
-        <v>0.00136</v>
+        <v>0.00145</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
@@ -1318,7 +1318,7 @@
         </is>
       </c>
       <c r="N14" t="n">
-        <v>0.00077</v>
+        <v>0.00076</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="Q14" t="n">
-        <v>0</v>
+        <v>1e-05</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="W14" t="n">
-        <v>0.00114</v>
+        <v>0.00108</v>
       </c>
     </row>
     <row r="15">
@@ -1360,7 +1360,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.00322</v>
+        <v>0.00354</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1368,7 +1368,7 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>0.00018</v>
+        <v>0.00016</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1376,7 +1376,7 @@
         </is>
       </c>
       <c r="K15" t="n">
-        <v>0.00353</v>
+        <v>0.00413</v>
       </c>
       <c r="M15" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         </is>
       </c>
       <c r="N15" t="n">
-        <v>0.00586</v>
+        <v>0.00613</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>
@@ -1408,7 +1408,7 @@
         </is>
       </c>
       <c r="W15" t="n">
-        <v>8.000000000000001e-05</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="16">
@@ -1418,7 +1418,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.00055</v>
+        <v>0.00058</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.00011</v>
+        <v>8.000000000000001e-05</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1434,7 +1434,7 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>0.00012</v>
+        <v>0.0003</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1474,7 +1474,7 @@
         </is>
       </c>
       <c r="W16" t="n">
-        <v>0</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="17">
@@ -1484,7 +1484,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.0019</v>
+        <v>0.00192</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.00154</v>
+        <v>0.0016</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1500,7 +1500,7 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>0.00074</v>
+        <v>0.00073</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1516,7 +1516,7 @@
         </is>
       </c>
       <c r="N17" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
@@ -1524,7 +1524,7 @@
         </is>
       </c>
       <c r="Q17" t="n">
-        <v>0.00018</v>
+        <v>0.0002</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
@@ -1550,7 +1550,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.0048</v>
+        <v>0.00479</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1566,7 +1566,7 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>0.00232</v>
+        <v>0.00239</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1574,7 +1574,7 @@
         </is>
       </c>
       <c r="K18" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>8.000000000000001e-05</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
@@ -1616,7 +1616,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.00464</v>
+        <v>0.00465</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1648,7 +1648,7 @@
         </is>
       </c>
       <c r="N19" t="n">
-        <v>0.0005</v>
+        <v>0.00049</v>
       </c>
       <c r="P19" t="inlineStr">
         <is>
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="W19" t="n">
-        <v>9.000000000000001e-05</v>
+        <v>0.00011</v>
       </c>
     </row>
     <row r="20">
@@ -1682,7 +1682,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>6e-05</v>
+        <v>5e-05</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.0014</v>
+        <v>0.00141</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1706,7 +1706,7 @@
         </is>
       </c>
       <c r="K20" t="n">
-        <v>0.00199</v>
+        <v>0.00201</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
@@ -1714,7 +1714,7 @@
         </is>
       </c>
       <c r="N20" t="n">
-        <v>0.00263</v>
+        <v>0.00267</v>
       </c>
       <c r="P20" t="inlineStr">
         <is>
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="Q20" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>9.000000000000001e-05</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
@@ -1738,7 +1738,7 @@
         </is>
       </c>
       <c r="W20" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1748,7 +1748,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.00124</v>
+        <v>0.00125</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1814,7 +1814,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.00063</v>
+        <v>0.00079</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1830,7 +1830,7 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>0.00169</v>
+        <v>0.00174</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1880,7 +1880,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>6e-05</v>
+        <v>6.999999999999999e-05</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -2210,7 +2210,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -2234,7 +2234,7 @@
         </is>
       </c>
       <c r="K28" t="n">
-        <v>0.00036</v>
+        <v>0.00045</v>
       </c>
       <c r="M28" t="inlineStr">
         <is>
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2382,7 +2382,7 @@
         </is>
       </c>
       <c r="Q30" t="n">
-        <v>0</v>
+        <v>1e-05</v>
       </c>
       <c r="S30" t="inlineStr">
         <is>
@@ -2482,7 +2482,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0.00074</v>
+        <v>0.00073</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -2490,7 +2490,7 @@
         </is>
       </c>
       <c r="H32" t="n">
-        <v>0.00141</v>
+        <v>0.00142</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2498,7 +2498,7 @@
         </is>
       </c>
       <c r="K32" t="n">
-        <v>0.00051</v>
+        <v>0.0005</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
@@ -2506,7 +2506,7 @@
         </is>
       </c>
       <c r="N32" t="n">
-        <v>0.00078</v>
+        <v>0.00077</v>
       </c>
       <c r="P32" t="inlineStr">
         <is>
@@ -2564,7 +2564,7 @@
         </is>
       </c>
       <c r="K33" t="n">
-        <v>0.01131</v>
+        <v>0.01187</v>
       </c>
       <c r="M33" t="inlineStr">
         <is>
@@ -2572,7 +2572,7 @@
         </is>
       </c>
       <c r="N33" t="n">
-        <v>0.00087</v>
+        <v>0.0008899999999999999</v>
       </c>
       <c r="P33" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
         </is>
       </c>
       <c r="T33" t="n">
-        <v>0.00051</v>
+        <v>0.0005</v>
       </c>
       <c r="V33" t="inlineStr">
         <is>
@@ -2638,7 +2638,7 @@
         </is>
       </c>
       <c r="N34" t="n">
-        <v>3e-05</v>
+        <v>4e-05</v>
       </c>
       <c r="P34" t="inlineStr">
         <is>
@@ -2680,7 +2680,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0.00115</v>
+        <v>0.00122</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -2704,7 +2704,7 @@
         </is>
       </c>
       <c r="N35" t="n">
-        <v>0.00151</v>
+        <v>0.00152</v>
       </c>
       <c r="P35" t="inlineStr">
         <is>
@@ -2746,7 +2746,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0.00342</v>
+        <v>0.00344</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -2754,7 +2754,7 @@
         </is>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>3e-05</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -2762,7 +2762,7 @@
         </is>
       </c>
       <c r="K36" t="n">
-        <v>0.00019</v>
+        <v>0.0002</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
@@ -2778,7 +2778,7 @@
         </is>
       </c>
       <c r="Q36" t="n">
-        <v>0</v>
+        <v>1e-05</v>
       </c>
       <c r="S36" t="inlineStr">
         <is>
@@ -2794,7 +2794,7 @@
         </is>
       </c>
       <c r="W36" t="n">
-        <v>2e-05</v>
+        <v>3e-05</v>
       </c>
     </row>
     <row r="37">
@@ -2820,7 +2820,7 @@
         </is>
       </c>
       <c r="H37" t="n">
-        <v>0.00022</v>
+        <v>0.00023</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -2870,7 +2870,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.00213</v>
+        <v>0.0023</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -2878,7 +2878,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0.00118</v>
+        <v>0.0012</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -2894,7 +2894,7 @@
         </is>
       </c>
       <c r="K38" t="n">
-        <v>0.007860000000000001</v>
+        <v>0.00825</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
@@ -2902,7 +2902,7 @@
         </is>
       </c>
       <c r="N38" t="n">
-        <v>0.00295</v>
+        <v>0.00302</v>
       </c>
       <c r="P38" t="inlineStr">
         <is>
@@ -2944,7 +2944,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.00076</v>
+        <v>0.00098</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -3076,7 +3076,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0.00011</v>
+        <v>0.00012</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -3084,7 +3084,7 @@
         </is>
       </c>
       <c r="H41" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3092,7 +3092,7 @@
         </is>
       </c>
       <c r="K41" t="n">
-        <v>0.0071</v>
+        <v>0.00729</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
@@ -3100,7 +3100,7 @@
         </is>
       </c>
       <c r="N41" t="n">
-        <v>0.00219</v>
+        <v>0.00224</v>
       </c>
       <c r="P41" t="inlineStr">
         <is>
@@ -3142,7 +3142,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0.00205</v>
+        <v>0.00206</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -3208,7 +3208,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.00102</v>
+        <v>0.00106</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -3216,7 +3216,7 @@
         </is>
       </c>
       <c r="H43" t="n">
-        <v>5e-05</v>
+        <v>0.00011</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3224,7 +3224,7 @@
         </is>
       </c>
       <c r="K43" t="n">
-        <v>0.00048</v>
+        <v>0.00049</v>
       </c>
       <c r="M43" t="inlineStr">
         <is>
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="N43" t="n">
-        <v>0.00452</v>
+        <v>0.00462</v>
       </c>
       <c r="P43" t="inlineStr">
         <is>
@@ -3266,7 +3266,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.00068</v>
+        <v>0.00069</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -3282,7 +3282,7 @@
         </is>
       </c>
       <c r="H44" t="n">
-        <v>0.00073</v>
+        <v>0.00072</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -3290,7 +3290,7 @@
         </is>
       </c>
       <c r="K44" t="n">
-        <v>0.00026</v>
+        <v>0.00025</v>
       </c>
       <c r="M44" t="inlineStr">
         <is>
@@ -3298,7 +3298,7 @@
         </is>
       </c>
       <c r="N44" t="n">
-        <v>0.00209</v>
+        <v>0.0021</v>
       </c>
       <c r="P44" t="inlineStr">
         <is>
@@ -3322,7 +3322,7 @@
         </is>
       </c>
       <c r="W44" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0.00013</v>
       </c>
     </row>
     <row r="45">
@@ -3340,7 +3340,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0.00322</v>
+        <v>0.00326</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         </is>
       </c>
       <c r="H45" t="n">
-        <v>4e-05</v>
+        <v>5e-05</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3364,7 +3364,7 @@
         </is>
       </c>
       <c r="N45" t="n">
-        <v>0.00109</v>
+        <v>0.00111</v>
       </c>
       <c r="P45" t="inlineStr">
         <is>
@@ -3406,7 +3406,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0.00667</v>
+        <v>0.00658</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -3414,7 +3414,7 @@
         </is>
       </c>
       <c r="H46" t="n">
-        <v>0.00077</v>
+        <v>0.0007</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -3422,7 +3422,7 @@
         </is>
       </c>
       <c r="K46" t="n">
-        <v>0.00413</v>
+        <v>0.00411</v>
       </c>
       <c r="M46" t="inlineStr">
         <is>
@@ -3430,7 +3430,7 @@
         </is>
       </c>
       <c r="N46" t="n">
-        <v>0.00057</v>
+        <v>0.00058</v>
       </c>
       <c r="P46" t="inlineStr">
         <is>
@@ -3454,7 +3454,7 @@
         </is>
       </c>
       <c r="W46" t="n">
-        <v>5e-05</v>
+        <v>8.000000000000001e-05</v>
       </c>
     </row>
     <row r="47">
@@ -3464,7 +3464,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.00136</v>
+        <v>0.00215</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -3472,7 +3472,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.00029</v>
+        <v>0.00033</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -3480,7 +3480,7 @@
         </is>
       </c>
       <c r="H47" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -3488,7 +3488,7 @@
         </is>
       </c>
       <c r="K47" t="n">
-        <v>0.00808</v>
+        <v>0.00844</v>
       </c>
       <c r="M47" t="inlineStr">
         <is>
@@ -3496,7 +3496,7 @@
         </is>
       </c>
       <c r="N47" t="n">
-        <v>0.00177</v>
+        <v>0.00197</v>
       </c>
       <c r="P47" t="inlineStr">
         <is>
@@ -3504,7 +3504,7 @@
         </is>
       </c>
       <c r="Q47" t="n">
-        <v>0.00259</v>
+        <v>0.00271</v>
       </c>
       <c r="S47" t="inlineStr">
         <is>
@@ -3538,7 +3538,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0.00053</v>
+        <v>0.00056</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -3546,7 +3546,7 @@
         </is>
       </c>
       <c r="H48" t="n">
-        <v>0</v>
+        <v>1e-05</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
         </is>
       </c>
       <c r="N48" t="n">
-        <v>0.00199</v>
+        <v>0.00201</v>
       </c>
       <c r="P48" t="inlineStr">
         <is>
@@ -3604,7 +3604,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0.00648</v>
+        <v>0.00647</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
         </is>
       </c>
       <c r="H49" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
         </is>
       </c>
       <c r="N49" t="n">
-        <v>6e-05</v>
+        <v>6.999999999999999e-05</v>
       </c>
       <c r="P49" t="inlineStr">
         <is>
@@ -3652,7 +3652,7 @@
         </is>
       </c>
       <c r="W49" t="n">
-        <v>0</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="50">
@@ -3670,7 +3670,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.00354</v>
+        <v>0.00355</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -3744,7 +3744,7 @@
         </is>
       </c>
       <c r="H51" t="n">
-        <v>0.00061</v>
+        <v>0.00062</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -3760,7 +3760,7 @@
         </is>
       </c>
       <c r="N51" t="n">
-        <v>0.009090000000000001</v>
+        <v>0.009339999999999999</v>
       </c>
       <c r="P51" t="inlineStr">
         <is>
@@ -3784,7 +3784,7 @@
         </is>
       </c>
       <c r="W51" t="n">
-        <v>0.00196</v>
+        <v>0.00219</v>
       </c>
     </row>
     <row r="52">
@@ -3794,7 +3794,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.00152</v>
+        <v>0.00156</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -3818,7 +3818,7 @@
         </is>
       </c>
       <c r="K52" t="n">
-        <v>0.0027</v>
+        <v>0.00293</v>
       </c>
       <c r="M52" t="inlineStr">
         <is>
@@ -4198,7 +4198,7 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>0.00076</v>
+        <v>0.00078</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -4322,7 +4322,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.0032</v>
+        <v>0.00321</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -4346,7 +4346,7 @@
         </is>
       </c>
       <c r="K60" t="n">
-        <v>0.00295</v>
+        <v>0.00297</v>
       </c>
       <c r="M60" t="inlineStr">
         <is>
@@ -4354,7 +4354,7 @@
         </is>
       </c>
       <c r="N60" t="n">
-        <v>0.00046</v>
+        <v>0.00048</v>
       </c>
       <c r="P60" t="inlineStr">
         <is>
@@ -4396,7 +4396,7 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>2e-05</v>
+        <v>0</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -4404,7 +4404,7 @@
         </is>
       </c>
       <c r="H61" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -4420,7 +4420,7 @@
         </is>
       </c>
       <c r="N61" t="n">
-        <v>0.00307</v>
+        <v>0.00306</v>
       </c>
       <c r="P61" t="inlineStr">
         <is>
@@ -4618,7 +4618,7 @@
         </is>
       </c>
       <c r="N64" t="n">
-        <v>0.00265</v>
+        <v>0.00264</v>
       </c>
       <c r="P64" t="inlineStr">
         <is>
@@ -4652,7 +4652,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.00524</v>
+        <v>0.00592</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -4668,7 +4668,7 @@
         </is>
       </c>
       <c r="H65" t="n">
-        <v>0.00727</v>
+        <v>0.00767</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -4684,7 +4684,7 @@
         </is>
       </c>
       <c r="N65" t="n">
-        <v>0.00457</v>
+        <v>0.0047</v>
       </c>
       <c r="P65" t="inlineStr">
         <is>
@@ -4742,7 +4742,7 @@
         </is>
       </c>
       <c r="K66" t="n">
-        <v>0.00334</v>
+        <v>0.00337</v>
       </c>
       <c r="M66" t="inlineStr">
         <is>
@@ -4816,7 +4816,7 @@
         </is>
       </c>
       <c r="N67" t="n">
-        <v>0.00204</v>
+        <v>0.00205</v>
       </c>
       <c r="P67" t="inlineStr">
         <is>
@@ -4840,7 +4840,7 @@
         </is>
       </c>
       <c r="W67" t="n">
-        <v>0</v>
+        <v>3e-05</v>
       </c>
     </row>
     <row r="68">
@@ -4866,7 +4866,7 @@
         </is>
       </c>
       <c r="H68" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -4874,7 +4874,7 @@
         </is>
       </c>
       <c r="K68" t="n">
-        <v>0.00449</v>
+        <v>0.00455</v>
       </c>
       <c r="M68" t="inlineStr">
         <is>
@@ -4906,7 +4906,7 @@
         </is>
       </c>
       <c r="W68" t="n">
-        <v>0</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="69">
@@ -4916,7 +4916,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.00017</v>
+        <v>0.0002</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -4924,7 +4924,7 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>0.00066</v>
+        <v>0.00067</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -4940,7 +4940,7 @@
         </is>
       </c>
       <c r="K69" t="n">
-        <v>0.0046</v>
+        <v>0.00467</v>
       </c>
       <c r="M69" t="inlineStr">
         <is>
@@ -4982,7 +4982,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.00467</v>
+        <v>0.00495</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -5014,7 +5014,7 @@
         </is>
       </c>
       <c r="N70" t="n">
-        <v>0.0049</v>
+        <v>0.00496</v>
       </c>
       <c r="P70" t="inlineStr">
         <is>
@@ -5022,7 +5022,7 @@
         </is>
       </c>
       <c r="Q70" t="n">
-        <v>0.0009300000000000001</v>
+        <v>0.00094</v>
       </c>
       <c r="S70" t="inlineStr">
         <is>
@@ -5038,7 +5038,7 @@
         </is>
       </c>
       <c r="W70" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -5056,7 +5056,7 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -5138,7 +5138,7 @@
         </is>
       </c>
       <c r="K72" t="n">
-        <v>0.00072</v>
+        <v>0.00073</v>
       </c>
       <c r="M72" t="inlineStr">
         <is>
@@ -5180,7 +5180,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.00333</v>
+        <v>0.00348</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -5196,7 +5196,7 @@
         </is>
       </c>
       <c r="H73" t="n">
-        <v>0.00188</v>
+        <v>0.00203</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -5204,7 +5204,7 @@
         </is>
       </c>
       <c r="K73" t="n">
-        <v>0.0008899999999999999</v>
+        <v>0.00091</v>
       </c>
       <c r="M73" t="inlineStr">
         <is>
@@ -5220,7 +5220,7 @@
         </is>
       </c>
       <c r="Q73" t="n">
-        <v>0.00031</v>
+        <v>0.00032</v>
       </c>
       <c r="S73" t="inlineStr">
         <is>
@@ -5270,7 +5270,7 @@
         </is>
       </c>
       <c r="K74" t="n">
-        <v>0.00378</v>
+        <v>0.00377</v>
       </c>
       <c r="M74" t="inlineStr">
         <is>
@@ -5320,7 +5320,7 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0.00011</v>
+        <v>0.00012</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -5336,7 +5336,7 @@
         </is>
       </c>
       <c r="K75" t="n">
-        <v>0.00176</v>
+        <v>0.00177</v>
       </c>
       <c r="M75" t="inlineStr">
         <is>
@@ -5368,7 +5368,7 @@
         </is>
       </c>
       <c r="W75" t="n">
-        <v>1e-05</v>
+        <v>3e-05</v>
       </c>
     </row>
     <row r="76">
@@ -5378,7 +5378,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.00108</v>
+        <v>0.00116</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -5394,7 +5394,7 @@
         </is>
       </c>
       <c r="H76" t="n">
-        <v>0.00052</v>
+        <v>0.00054</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -5402,7 +5402,7 @@
         </is>
       </c>
       <c r="K76" t="n">
-        <v>0.00547</v>
+        <v>0.00557</v>
       </c>
       <c r="M76" t="inlineStr">
         <is>
@@ -5410,7 +5410,7 @@
         </is>
       </c>
       <c r="N76" t="n">
-        <v>0.0003</v>
+        <v>0.00029</v>
       </c>
       <c r="P76" t="inlineStr">
         <is>
@@ -5468,7 +5468,7 @@
         </is>
       </c>
       <c r="K77" t="n">
-        <v>0.00424</v>
+        <v>0.00423</v>
       </c>
       <c r="M77" t="inlineStr">
         <is>
@@ -5476,7 +5476,7 @@
         </is>
       </c>
       <c r="N77" t="n">
-        <v>2e-05</v>
+        <v>3e-05</v>
       </c>
       <c r="P77" t="inlineStr">
         <is>
@@ -5500,7 +5500,7 @@
         </is>
       </c>
       <c r="W77" t="n">
-        <v>8.000000000000001e-05</v>
+        <v>0.00011</v>
       </c>
     </row>
     <row r="78">
@@ -5526,7 +5526,7 @@
         </is>
       </c>
       <c r="H78" t="n">
-        <v>0.00287</v>
+        <v>0.00345</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -5534,7 +5534,7 @@
         </is>
       </c>
       <c r="K78" t="n">
-        <v>0.00646</v>
+        <v>0.00765</v>
       </c>
       <c r="M78" t="inlineStr">
         <is>
@@ -5542,7 +5542,7 @@
         </is>
       </c>
       <c r="N78" t="n">
-        <v>0.00123</v>
+        <v>0.00122</v>
       </c>
       <c r="P78" t="inlineStr">
         <is>
@@ -5566,7 +5566,7 @@
         </is>
       </c>
       <c r="W78" t="n">
-        <v>5e-05</v>
+        <v>3e-05</v>
       </c>
     </row>
     <row r="79">
@@ -5576,7 +5576,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.00579</v>
+        <v>0.00615</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -5584,7 +5584,7 @@
         </is>
       </c>
       <c r="E79" t="n">
-        <v>1e-05</v>
+        <v>3e-05</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -5592,7 +5592,7 @@
         </is>
       </c>
       <c r="H79" t="n">
-        <v>0.00674</v>
+        <v>0.00685</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -5600,7 +5600,7 @@
         </is>
       </c>
       <c r="K79" t="n">
-        <v>0.00018</v>
+        <v>0.00021</v>
       </c>
       <c r="M79" t="inlineStr">
         <is>
@@ -5608,7 +5608,7 @@
         </is>
       </c>
       <c r="N79" t="n">
-        <v>0.01192</v>
+        <v>0.0122</v>
       </c>
       <c r="P79" t="inlineStr">
         <is>
@@ -5642,7 +5642,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.0001</v>
+        <v>0.00013</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -5666,7 +5666,7 @@
         </is>
       </c>
       <c r="K80" t="n">
-        <v>0.00111</v>
+        <v>0.00113</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
@@ -5698,7 +5698,7 @@
         </is>
       </c>
       <c r="W80" t="n">
-        <v>0</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="81">
@@ -5724,7 +5724,7 @@
         </is>
       </c>
       <c r="H81" t="n">
-        <v>0.00164</v>
+        <v>0.00169</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -5740,7 +5740,7 @@
         </is>
       </c>
       <c r="N81" t="n">
-        <v>0.00248</v>
+        <v>0.00251</v>
       </c>
       <c r="P81" t="inlineStr">
         <is>
@@ -5774,7 +5774,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.00263</v>
+        <v>0.00303</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -5790,7 +5790,7 @@
         </is>
       </c>
       <c r="H82" t="n">
-        <v>4e-05</v>
+        <v>5e-05</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -5798,7 +5798,7 @@
         </is>
       </c>
       <c r="K82" t="n">
-        <v>0.00571</v>
+        <v>0.00577</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
@@ -5806,7 +5806,7 @@
         </is>
       </c>
       <c r="N82" t="n">
-        <v>0.00071</v>
+        <v>0.0007</v>
       </c>
       <c r="P82" t="inlineStr">
         <is>
@@ -5856,7 +5856,7 @@
         </is>
       </c>
       <c r="H83" t="n">
-        <v>0.00053</v>
+        <v>0.00055</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -5864,7 +5864,7 @@
         </is>
       </c>
       <c r="K83" t="n">
-        <v>0.00651</v>
+        <v>0.00654</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
@@ -5896,7 +5896,7 @@
         </is>
       </c>
       <c r="W83" t="n">
-        <v>0.00023</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="84">
@@ -5906,7 +5906,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.0006400000000000001</v>
+        <v>0.00065</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -5922,7 +5922,7 @@
         </is>
       </c>
       <c r="H84" t="n">
-        <v>0.001</v>
+        <v>0.00112</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -5938,7 +5938,7 @@
         </is>
       </c>
       <c r="N84" t="n">
-        <v>0.00075</v>
+        <v>0.00078</v>
       </c>
       <c r="P84" t="inlineStr">
         <is>
@@ -5962,7 +5962,7 @@
         </is>
       </c>
       <c r="W84" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -5996,7 +5996,7 @@
         </is>
       </c>
       <c r="K85" t="n">
-        <v>0.00012</v>
+        <v>0.00018</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
@@ -6194,7 +6194,7 @@
         </is>
       </c>
       <c r="K88" t="n">
-        <v>0.00128</v>
+        <v>0.00136</v>
       </c>
       <c r="M88" t="inlineStr">
         <is>
@@ -6358,7 +6358,7 @@
         </is>
       </c>
       <c r="W90" t="n">
-        <v>0.00026</v>
+        <v>0.00025</v>
       </c>
     </row>
     <row r="91">
@@ -6434,7 +6434,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.00289</v>
+        <v>0.00315</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -6458,7 +6458,7 @@
         </is>
       </c>
       <c r="K92" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
       <c r="M92" t="inlineStr">
         <is>
@@ -6466,7 +6466,7 @@
         </is>
       </c>
       <c r="N92" t="n">
-        <v>0.00149</v>
+        <v>0.00157</v>
       </c>
       <c r="P92" t="inlineStr">
         <is>
@@ -6532,7 +6532,7 @@
         </is>
       </c>
       <c r="N93" t="n">
-        <v>0.00559</v>
+        <v>0.00558</v>
       </c>
       <c r="P93" t="inlineStr">
         <is>
@@ -6556,7 +6556,7 @@
         </is>
       </c>
       <c r="W93" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -6640,7 +6640,7 @@
         </is>
       </c>
       <c r="E95" t="n">
-        <v>0</v>
+        <v>1e-05</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -6764,7 +6764,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.00114</v>
+        <v>0.00117</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -6772,7 +6772,7 @@
         </is>
       </c>
       <c r="E97" t="n">
-        <v>0.00591</v>
+        <v>0.00596</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -6788,7 +6788,7 @@
         </is>
       </c>
       <c r="K97" t="n">
-        <v>0.0007</v>
+        <v>0.00124</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
@@ -6796,7 +6796,7 @@
         </is>
       </c>
       <c r="N97" t="n">
-        <v>2e-05</v>
+        <v>3e-05</v>
       </c>
       <c r="P97" t="inlineStr">
         <is>
@@ -6820,7 +6820,7 @@
         </is>
       </c>
       <c r="W97" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -6878,7 +6878,7 @@
         </is>
       </c>
       <c r="T98" t="n">
-        <v>0.00101</v>
+        <v>0.001</v>
       </c>
       <c r="V98" t="inlineStr">
         <is>
@@ -6896,7 +6896,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>8.000000000000001e-05</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -6928,7 +6928,7 @@
         </is>
       </c>
       <c r="N99" t="n">
-        <v>0.00044</v>
+        <v>0.00047</v>
       </c>
       <c r="P99" t="inlineStr">
         <is>
@@ -6952,7 +6952,7 @@
         </is>
       </c>
       <c r="W99" t="n">
-        <v>0.00013</v>
+        <v>0.00014</v>
       </c>
     </row>
     <row r="100">
@@ -6994,7 +6994,7 @@
         </is>
       </c>
       <c r="N100" t="n">
-        <v>0.00106</v>
+        <v>0.00113</v>
       </c>
       <c r="P100" t="inlineStr">
         <is>
@@ -7010,7 +7010,7 @@
         </is>
       </c>
       <c r="T100" t="n">
-        <v>0.00015</v>
+        <v>0.00016</v>
       </c>
       <c r="V100" t="inlineStr">
         <is>
@@ -7036,7 +7036,7 @@
         </is>
       </c>
       <c r="E101" t="n">
-        <v>0.00068</v>
+        <v>0.00074</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -7060,7 +7060,7 @@
         </is>
       </c>
       <c r="N101" t="n">
-        <v>0.0017</v>
+        <v>0.00172</v>
       </c>
       <c r="P101" t="inlineStr">
         <is>
@@ -7094,7 +7094,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.00032</v>
+        <v>0.00035</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -7110,7 +7110,7 @@
         </is>
       </c>
       <c r="H102" t="n">
-        <v>0.00287</v>
+        <v>0.00299</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
@@ -7118,7 +7118,7 @@
         </is>
       </c>
       <c r="K102" t="n">
-        <v>0.00161</v>
+        <v>0.00187</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
@@ -7126,7 +7126,7 @@
         </is>
       </c>
       <c r="N102" t="n">
-        <v>8.000000000000001e-05</v>
+        <v>6e-05</v>
       </c>
       <c r="P102" t="inlineStr">
         <is>
@@ -7134,7 +7134,7 @@
         </is>
       </c>
       <c r="Q102" t="n">
-        <v>0.00302</v>
+        <v>0.00308</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
@@ -7150,7 +7150,7 @@
         </is>
       </c>
       <c r="W102" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="103">
@@ -7192,7 +7192,7 @@
         </is>
       </c>
       <c r="N103" t="n">
-        <v>0.00143</v>
+        <v>0.00147</v>
       </c>
       <c r="P103" t="inlineStr">
         <is>
@@ -7308,7 +7308,7 @@
         </is>
       </c>
       <c r="H105" t="n">
-        <v>0.00584</v>
+        <v>0.00588</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
@@ -7316,7 +7316,7 @@
         </is>
       </c>
       <c r="K105" t="n">
-        <v>0.00034</v>
+        <v>0.00035</v>
       </c>
       <c r="M105" t="inlineStr">
         <is>
@@ -7348,7 +7348,7 @@
         </is>
       </c>
       <c r="W105" t="n">
-        <v>2e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="106">
@@ -7456,7 +7456,7 @@
         </is>
       </c>
       <c r="N107" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.00061</v>
       </c>
       <c r="P107" t="inlineStr">
         <is>
@@ -7472,7 +7472,7 @@
         </is>
       </c>
       <c r="T107" t="n">
-        <v>0.00023</v>
+        <v>0.00024</v>
       </c>
       <c r="V107" t="inlineStr">
         <is>
@@ -7480,7 +7480,7 @@
         </is>
       </c>
       <c r="W107" t="n">
-        <v>4e-05</v>
+        <v>0.00013</v>
       </c>
     </row>
     <row r="108">
@@ -7490,7 +7490,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.00136</v>
+        <v>0.00153</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
@@ -7522,7 +7522,7 @@
         </is>
       </c>
       <c r="N108" t="n">
-        <v>0.00216</v>
+        <v>0.0021</v>
       </c>
       <c r="P108" t="inlineStr">
         <is>
@@ -7556,7 +7556,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0</v>
+        <v>6e-05</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
@@ -7630,7 +7630,7 @@
         </is>
       </c>
       <c r="E110" t="n">
-        <v>0.00177</v>
+        <v>0.00184</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
@@ -7654,7 +7654,7 @@
         </is>
       </c>
       <c r="N110" t="n">
-        <v>0.00026</v>
+        <v>0.00021</v>
       </c>
       <c r="P110" t="inlineStr">
         <is>
@@ -7670,7 +7670,7 @@
         </is>
       </c>
       <c r="T110" t="n">
-        <v>0.00054</v>
+        <v>0.00051</v>
       </c>
       <c r="V110" t="inlineStr">
         <is>
@@ -7678,7 +7678,7 @@
         </is>
       </c>
       <c r="W110" t="n">
-        <v>0.00074</v>
+        <v>0.00069</v>
       </c>
     </row>
     <row r="111">
@@ -7688,7 +7688,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.008829999999999999</v>
+        <v>0.008970000000000001</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -7712,7 +7712,7 @@
         </is>
       </c>
       <c r="K111" t="n">
-        <v>0.00764</v>
+        <v>0.00795</v>
       </c>
       <c r="M111" t="inlineStr">
         <is>
@@ -7720,7 +7720,7 @@
         </is>
       </c>
       <c r="N111" t="n">
-        <v>6e-05</v>
+        <v>5e-05</v>
       </c>
       <c r="P111" t="inlineStr">
         <is>
@@ -7728,7 +7728,7 @@
         </is>
       </c>
       <c r="Q111" t="n">
-        <v>1e-05</v>
+        <v>3e-05</v>
       </c>
       <c r="S111" t="inlineStr">
         <is>
@@ -7736,7 +7736,7 @@
         </is>
       </c>
       <c r="T111" t="n">
-        <v>1e-05</v>
+        <v>2e-05</v>
       </c>
       <c r="V111" t="inlineStr">
         <is>
@@ -7786,7 +7786,7 @@
         </is>
       </c>
       <c r="N112" t="n">
-        <v>0.00032</v>
+        <v>0.00035</v>
       </c>
       <c r="P112" t="inlineStr">
         <is>
@@ -7810,7 +7810,7 @@
         </is>
       </c>
       <c r="W112" t="n">
-        <v>3e-05</v>
+        <v>5e-05</v>
       </c>
     </row>
     <row r="113">
@@ -7820,7 +7820,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.00179</v>
+        <v>0.00198</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -7844,7 +7844,7 @@
         </is>
       </c>
       <c r="K113" t="n">
-        <v>0.00602</v>
+        <v>0.00617</v>
       </c>
       <c r="M113" t="inlineStr">
         <is>
@@ -7876,7 +7876,7 @@
         </is>
       </c>
       <c r="W113" t="n">
-        <v>2e-05</v>
+        <v>3e-05</v>
       </c>
     </row>
     <row r="114">
@@ -7910,7 +7910,7 @@
         </is>
       </c>
       <c r="K114" t="n">
-        <v>0</v>
+        <v>1e-05</v>
       </c>
       <c r="M114" t="inlineStr">
         <is>
@@ -7918,7 +7918,7 @@
         </is>
       </c>
       <c r="N114" t="n">
-        <v>0.0009700000000000001</v>
+        <v>0.00103</v>
       </c>
       <c r="P114" t="inlineStr">
         <is>
@@ -7934,7 +7934,7 @@
         </is>
       </c>
       <c r="T114" t="n">
-        <v>0.00043</v>
+        <v>0.00044</v>
       </c>
       <c r="V114" t="inlineStr">
         <is>
@@ -7942,7 +7942,7 @@
         </is>
       </c>
       <c r="W114" t="n">
-        <v>0.00081</v>
+        <v>0.0008</v>
       </c>
     </row>
     <row r="115">
@@ -7968,7 +7968,7 @@
         </is>
       </c>
       <c r="H115" t="n">
-        <v>2e-05</v>
+        <v>3e-05</v>
       </c>
       <c r="J115" t="inlineStr">
         <is>
@@ -7984,7 +7984,7 @@
         </is>
       </c>
       <c r="N115" t="n">
-        <v>0.00102</v>
+        <v>0.00099</v>
       </c>
       <c r="P115" t="inlineStr">
         <is>
@@ -7992,7 +7992,7 @@
         </is>
       </c>
       <c r="Q115" t="n">
-        <v>0.00299</v>
+        <v>0.00323</v>
       </c>
       <c r="S115" t="inlineStr">
         <is>
@@ -8000,7 +8000,7 @@
         </is>
       </c>
       <c r="T115" t="n">
-        <v>0.00042</v>
+        <v>0.00041</v>
       </c>
       <c r="V115" t="inlineStr">
         <is>
@@ -8034,7 +8034,7 @@
         </is>
       </c>
       <c r="H116" t="n">
-        <v>0.00095</v>
+        <v>0.00096</v>
       </c>
       <c r="J116" t="inlineStr">
         <is>
@@ -8042,7 +8042,7 @@
         </is>
       </c>
       <c r="K116" t="n">
-        <v>0.00048</v>
+        <v>0.0005</v>
       </c>
       <c r="M116" t="inlineStr">
         <is>
@@ -8140,7 +8140,7 @@
         </is>
       </c>
       <c r="W117" t="n">
-        <v>0</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="118">
@@ -8166,7 +8166,7 @@
         </is>
       </c>
       <c r="H118" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
       <c r="J118" t="inlineStr">
         <is>
@@ -8182,7 +8182,7 @@
         </is>
       </c>
       <c r="N118" t="n">
-        <v>0.00033</v>
+        <v>0.00032</v>
       </c>
       <c r="P118" t="inlineStr">
         <is>
@@ -8298,7 +8298,7 @@
         </is>
       </c>
       <c r="H120" t="n">
-        <v>0.00025</v>
+        <v>0.00024</v>
       </c>
       <c r="J120" t="inlineStr">
         <is>
@@ -8338,7 +8338,7 @@
         </is>
       </c>
       <c r="W120" t="n">
-        <v>6e-05</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="121">
@@ -8628,7 +8628,7 @@
         </is>
       </c>
       <c r="H125" t="n">
-        <v>0.00341</v>
+        <v>0.00342</v>
       </c>
       <c r="J125" t="inlineStr">
         <is>
@@ -8636,7 +8636,7 @@
         </is>
       </c>
       <c r="K125" t="n">
-        <v>4e-05</v>
+        <v>0.0013</v>
       </c>
       <c r="M125" t="inlineStr">
         <is>
@@ -8644,7 +8644,7 @@
         </is>
       </c>
       <c r="N125" t="n">
-        <v>1e-05</v>
+        <v>0</v>
       </c>
       <c r="P125" t="inlineStr">
         <is>
@@ -8668,7 +8668,7 @@
         </is>
       </c>
       <c r="W125" t="n">
-        <v>2e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -8760,7 +8760,7 @@
         </is>
       </c>
       <c r="H127" t="n">
-        <v>0.00067</v>
+        <v>0.00069</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>

</xml_diff>